<commit_message>
update ground truth on main.py, results "output.xlsx" has been updated
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ20"/>
+  <dimension ref="A1:AR20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,215 +436,220 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Input</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Jaccard Corrected</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>JaroDistance Corrected</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Dice Coefficien Corrected</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Cosine Corrected</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Damerau-Levenshtein Corrected</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Euclidien Distance Corrected</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Hamstring Distance Corrected</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>hamming Distance Corrected</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Jaro-Winkler Corrected</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Longest Common Corrected</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Levenshtein Distance Corrected</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Manhattan Corrected</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Needleman Corrected</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>N-Gram Corrected</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Smith Waterman Corrected</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Jaccard Time</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>JaroDistance Time</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Dice Coefficien Time</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Cosine Time</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Damerau-Levenshtein Time</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Euclidien Distance Time</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Hamstring Distance Time</t>
-        </is>
-      </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
+          <t>hamming Distance Time</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
           <t>Jaro-Winkler Time</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Longest Common Time</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Levenshtein Distance Time</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Manhattan Time</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Needleman Time</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>N-Gram Time</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Smith Waterman Time</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Jaccard Accuracy</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>JaroDistance Accuracy</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Dice Coefficien Accuracy</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Cosine Accuracy</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Damerau-Levenshtein Accuracy</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Euclidien Distance Accuracy</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Hamstring Distance Accuracy</t>
-        </is>
-      </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
+          <t>hamming Distance Accuracy</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
           <t>Jaro-Winkler Accuracy</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Longest Common Accuracy</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Levenshtein Distance Accuracy</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Manhattan Accuracy</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Needleman Accuracy</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>N-Gram Accuracy</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Smith Waterman Accuracy</t>
         </is>
@@ -653,2744 +658,2829 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>turn on the tea.</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the tea</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the the</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
+          <t>turn on the tv</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>turn on the enable</t>
-        </is>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
+          <t>turn on the tv</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>turn on the tv</t>
+        </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.0004992485046386719</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0004992485046386719</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0004992485046386719</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0004992485046386719</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0004992485046386719</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="V2" t="n">
-        <v>0.0004992485046386719</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="W2" t="n">
-        <v>0.001000642776489258</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="X2" t="n">
-        <v>0.001000642776489258</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.00118708610534668</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.001253843307495117</v>
+        <v>0.01084661483764648</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.001349449157714844</v>
+        <v>0.01182317733764648</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.001381397247314453</v>
+        <v>0.01182317733764648</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.001381397247314453</v>
+        <v>0.01182317733764648</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.6</v>
+        <v>0.01182317733764648</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.611111111111111</v>
+        <v>0.8703703703703703</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.8703703703703703</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>turn off the flight.</t>
+          <t>turn off the light</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>turn off the flight</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="P3" t="n">
-        <v>0.001381397247314453</v>
-      </c>
       <c r="Q3" t="n">
-        <v>0.001906633377075195</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="R3" t="n">
-        <v>0.002079248428344727</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="S3" t="n">
-        <v>0.002079248428344727</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="T3" t="n">
-        <v>0.0019683837890625</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="U3" t="n">
-        <v>0.002407073974609375</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="V3" t="n">
-        <v>0.002407073974609375</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="W3" t="n">
-        <v>0.002407073974609375</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="X3" t="n">
-        <v>0.002407073974609375</v>
+        <v>0.02137184143066406</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.002407073974609375</v>
+        <v>0.02234387397766113</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.00290679931640625</v>
+        <v>0.02331852912902832</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.00290679931640625</v>
+        <v>0.02331852912902832</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.00290679931640625</v>
+        <v>0.02331852912902832</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.003236532211303711</v>
+        <v>0.02331852912902832</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.02331852912902832</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9814814814814815</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0.9814814814814815</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>look the door.</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>lock the back door</t>
+          <t>look the door</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>lock the on</t>
+          <t>lock the door</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>lock the on</t>
-        </is>
-      </c>
-      <c r="P4" t="n">
-        <v>0.00812983512878418</v>
+          <t>lock the door</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>lock the door</t>
+        </is>
       </c>
       <c r="Q4" t="n">
-        <v>0.008241176605224609</v>
+        <v>0.02234458923339844</v>
       </c>
       <c r="R4" t="n">
-        <v>0.008533477783203125</v>
+        <v>0.02234458923339844</v>
       </c>
       <c r="S4" t="n">
-        <v>0.008668899536132812</v>
+        <v>0.02234458923339844</v>
       </c>
       <c r="T4" t="n">
-        <v>0.00845646858215332</v>
+        <v>0.02234458923339844</v>
       </c>
       <c r="U4" t="n">
-        <v>0.008994340896606445</v>
+        <v>0.02234458923339844</v>
       </c>
       <c r="V4" t="n">
-        <v>0.009154319763183594</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="W4" t="n">
-        <v>0.009249210357666016</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="X4" t="n">
-        <v>0.009249210357666016</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.009354352951049805</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.009480476379394531</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.009564638137817383</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.009629249572753906</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.01024079322814941</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.02284574508666992</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.7</v>
+        <v>0.875</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.7</v>
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0.9166666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>unluck the door.</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>unlock the back door</t>
+          <t>unluck the door</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
+          <t>unlock the door</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>unlock the on</t>
-        </is>
-      </c>
-      <c r="P5" t="n">
-        <v>0.01307272911071777</v>
+          <t>unlock the door</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>unlock the door</t>
+        </is>
       </c>
       <c r="Q5" t="n">
-        <v>0.01323461532592773</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0139153003692627</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0139153003692627</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="T5" t="n">
-        <v>0.01323461532592773</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0139153003692627</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="V5" t="n">
-        <v>0.0139153003692627</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="W5" t="n">
-        <v>0.01446008682250977</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="X5" t="n">
-        <v>0.01446008682250977</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.01508426666259766</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.01508426666259766</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.01537895202636719</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.0159914493560791</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.01600122451782227</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.02872991561889648</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0.7277777777777779</v>
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0.9444444444444444</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>turn on the lump.</t>
+          <t>turn on the lamp</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>turn on the lump</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="P6" t="n">
-        <v>0.008818149566650391</v>
-      </c>
       <c r="Q6" t="n">
-        <v>0.008818149566650391</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="R6" t="n">
-        <v>0.008818149566650391</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="S6" t="n">
-        <v>0.008818149566650391</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="T6" t="n">
-        <v>0.008818149566650391</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="U6" t="n">
-        <v>0.008818149566650391</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="V6" t="n">
-        <v>0.008818149566650391</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="W6" t="n">
-        <v>0.008818149566650391</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="X6" t="n">
-        <v>0.009586572647094727</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.009661436080932617</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.009661436080932617</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.009661436080932617</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.009661436080932617</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.009985446929931641</v>
+        <v>0.04895639419555664</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.5</v>
+        <v>0.04995179176330566</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.9444444444444445</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>look the windows.</t>
+          <t>lock the windows</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>look the windows</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="P7" t="n">
-        <v>0.02118468284606934</v>
-      </c>
       <c r="Q7" t="n">
-        <v>0.02136659622192383</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="R7" t="n">
-        <v>0.02148985862731934</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="S7" t="n">
-        <v>0.02183079719543457</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="T7" t="n">
-        <v>0.02148985862731934</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="U7" t="n">
-        <v>0.02188229560852051</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0225679874420166</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="W7" t="n">
-        <v>0.0225679874420166</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0228722095489502</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.02334165573120117</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.02334165573120117</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.02348637580871582</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.0239870548248291</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.02413225173950195</v>
+        <v>0.03751754760742188</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.8035714285714286</v>
+        <v>0.03849315643310547</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.875</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AQ7" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0.9166666666666667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>unluck the windows.</t>
+          <t>unlock the windows</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>unluck the windows</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="P8" t="n">
-        <v>0.02803444862365723</v>
-      </c>
       <c r="Q8" t="n">
-        <v>0.02803444862365723</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="R8" t="n">
-        <v>0.02901148796081543</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="S8" t="n">
-        <v>0.02901148796081543</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="T8" t="n">
-        <v>0.02901148796081543</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="U8" t="n">
-        <v>0.02901148796081543</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="V8" t="n">
-        <v>0.02901148796081543</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="W8" t="n">
-        <v>0.02901148796081543</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="X8" t="n">
-        <v>0.03102993965148926</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.03102993965148926</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.03121399879455566</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.03121399879455566</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.03155755996704102</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.0317223072052002</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.8452380952380952</v>
+        <v>0.04352903366088867</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AQ8" t="n">
-        <v>0.9236111111111112</v>
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0.9444444444444444</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>turn on the van.</t>
+          <t>turn on the fan</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>turn on the van</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="P9" t="n">
-        <v>0.01744461059570312</v>
-      </c>
       <c r="Q9" t="n">
-        <v>0.01755690574645996</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="R9" t="n">
-        <v>0.01768255233764648</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="S9" t="n">
-        <v>0.01768255233764648</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="T9" t="n">
-        <v>0.01761221885681152</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="U9" t="n">
-        <v>0.01768255233764648</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="V9" t="n">
-        <v>0.01768255233764648</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="W9" t="n">
-        <v>0.01795554161071777</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="X9" t="n">
-        <v>0.01795554161071777</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.01795554161071777</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.01819419860839844</v>
+        <v>0.07251381874084473</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.01819419860839844</v>
+        <v>0.0730125904083252</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.01819419860839844</v>
+        <v>0.0730125904083252</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.01840424537658691</v>
+        <v>0.0730125904083252</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.4</v>
+        <v>0.0730125904083252</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>turn off the van.</t>
+          <t>turn off the fan</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>turn off the van</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="P10" t="n">
-        <v>0.01845812797546387</v>
-      </c>
       <c r="Q10" t="n">
-        <v>0.01845812797546387</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="R10" t="n">
-        <v>0.01845812797546387</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="S10" t="n">
-        <v>0.01845812797546387</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="T10" t="n">
-        <v>0.01845812797546387</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="U10" t="n">
-        <v>0.01845812797546387</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="V10" t="n">
-        <v>0.01845812797546387</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="W10" t="n">
-        <v>0.01845812797546387</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="X10" t="n">
-        <v>0.01912856101989746</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.01918792724609375</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.01925253868103027</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.01931500434875488</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.01943111419677734</v>
+        <v>0.08415317535400391</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.01948213577270508</v>
+        <v>0.08536219596862793</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.4</v>
+        <v>0.08536219596862793</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AK10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AL10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AM10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AN10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AP10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="AQ10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9259259259259259</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>turn on the hater.</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the hater</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
+          <t>turn on the heater</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>turn on the gate</t>
-        </is>
-      </c>
-      <c r="P11" t="n">
-        <v>0.0195622444152832</v>
+          <t>turn on the heater</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>turn on the heater</t>
+        </is>
       </c>
       <c r="Q11" t="n">
-        <v>0.0195622444152832</v>
+        <v>0.09165453910827637</v>
       </c>
       <c r="R11" t="n">
-        <v>0.0195622444152832</v>
+        <v>0.09165453910827637</v>
       </c>
       <c r="S11" t="n">
-        <v>0.01996874809265137</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="T11" t="n">
-        <v>0.0195622444152832</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="U11" t="n">
-        <v>0.01996874809265137</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="V11" t="n">
-        <v>0.01996874809265137</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="W11" t="n">
-        <v>0.02033877372741699</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="X11" t="n">
-        <v>0.02033877372741699</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.02033877372741699</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.02033877372741699</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.02033877372741699</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.02080631256103516</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.02080631256103516</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.09262895584106445</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AM11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AN11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AP11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
       </c>
       <c r="AQ11" t="n">
-        <v>0.75</v>
+        <v>0.9592592592592593</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0.9592592592592593</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unable the hater.</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>unable the hater</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
+          <t>enable the heater</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>enable the gate</t>
-        </is>
-      </c>
-      <c r="P12" t="n">
-        <v>0.04299426078796387</v>
+          <t>enable the heater</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>enable the heater</t>
+        </is>
       </c>
       <c r="Q12" t="n">
-        <v>0.04360437393188477</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="R12" t="n">
-        <v>0.04385972023010254</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="S12" t="n">
-        <v>0.0439600944519043</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="T12" t="n">
-        <v>0.04370760917663574</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="U12" t="n">
-        <v>0.04441213607788086</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="V12" t="n">
-        <v>0.04441213607788086</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="W12" t="n">
-        <v>0.04441213607788086</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="X12" t="n">
-        <v>0.04472637176513672</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.04478359222412109</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.04529690742492676</v>
+        <v>0.06710195541381836</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.04536032676696777</v>
+        <v>0.06758332252502441</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.04542994499206543</v>
+        <v>0.06758332252502441</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.04542994499206543</v>
+        <v>0.06758332252502441</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.6309523809523809</v>
+        <v>0.06758332252502441</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AP12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
       </c>
       <c r="AQ12" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.8833333333333334</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0.8833333333333334</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>disassemble the back door.</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>disable the back door back door</t>
+          <t>disassemble the back door</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
+          <t>disable the back door</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>disable the back door on</t>
-        </is>
-      </c>
-      <c r="P13" t="n">
-        <v>0.07814574241638184</v>
+          <t>disable the back door</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>disable the back door</t>
+        </is>
       </c>
       <c r="Q13" t="n">
-        <v>0.07814574241638184</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="R13" t="n">
-        <v>0.07924008369445801</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="S13" t="n">
-        <v>0.07924008369445801</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="T13" t="n">
-        <v>0.07873916625976562</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="U13" t="n">
-        <v>0.08023715019226074</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="V13" t="n">
-        <v>0.08023715019226074</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="W13" t="n">
-        <v>0.08123683929443359</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="X13" t="n">
-        <v>0.08123683929443359</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.0823676586151123</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.08243060111999512</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.08252048492431641</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.08257865905761719</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.08347725868225098</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.109529972076416</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AK13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AL13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AM13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AN13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AO13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AP13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
       </c>
       <c r="AQ13" t="n">
-        <v>0.7375501042167709</v>
+        <v>0.9437229437229436</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0.9437229437229436</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>unluck the back door.</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>unlock the back door back door</t>
+          <t>unluck the back door</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
+          <t>unlock the back door</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>unlock the back door on</t>
-        </is>
-      </c>
-      <c r="P14" t="n">
-        <v>0.09287285804748535</v>
+          <t>unlock the back door</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>unlock the back door</t>
+        </is>
       </c>
       <c r="Q14" t="n">
-        <v>0.09344005584716797</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="R14" t="n">
-        <v>0.09376835823059082</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="S14" t="n">
-        <v>0.09376835823059082</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="T14" t="n">
-        <v>0.09376835823059082</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="U14" t="n">
-        <v>0.09376835823059082</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="V14" t="n">
-        <v>0.09529876708984375</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="W14" t="n">
-        <v>0.09541606903076172</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="X14" t="n">
-        <v>0.09558677673339844</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.09558677673339844</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.09558677673339844</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.09608793258666992</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.09608793258666992</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.09658908843994141</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.118302583694458</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AG14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AJ14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AK14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AL14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AM14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AN14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AO14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AP14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="AQ14" t="n">
-        <v>0.7567901234567902</v>
+        <v>0.9629629629629629</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>look the gate.</t>
+          <t>lock the gate</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>look the gate</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="P15" t="n">
-        <v>0.06941723823547363</v>
-      </c>
       <c r="Q15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="R15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="S15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="T15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="U15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="V15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="W15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="X15" t="n">
-        <v>0.06941723823547363</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.07019615173339844</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.07019615173339844</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.07120060920715332</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.07120060920715332</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.07120060920715332</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.775</v>
+        <v>0.08279895782470703</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.875</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AH15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AJ15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AK15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AL15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AM15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AN15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AO15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AP15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AQ15" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>0.9166666666666667</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>unluck the gate.</t>
+          <t>unlock the gate</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>unluck the gate</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="P16" t="n">
-        <v>0.07368183135986328</v>
-      </c>
       <c r="Q16" t="n">
-        <v>0.07368183135986328</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="R16" t="n">
-        <v>0.07418155670166016</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="S16" t="n">
-        <v>0.07418155670166016</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="T16" t="n">
-        <v>0.07418155670166016</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="U16" t="n">
-        <v>0.07418155670166016</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="V16" t="n">
-        <v>0.07418155670166016</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="W16" t="n">
-        <v>0.07418155670166016</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="X16" t="n">
-        <v>0.07523179054260254</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.07535433769226074</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.07535433769226074</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.07535433769226074</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.07535433769226074</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.07568120956420898</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.8166666666666667</v>
+        <v>0.09022045135498047</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AI16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AJ16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AK16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AL16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AM16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AN16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AO16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AP16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="AQ16" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>0.9444444444444444</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>turn on the over.</t>
+          <t>turn on the oven</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>turn on the over</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
+      <c r="O17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="P17" t="n">
-        <v>0.03812980651855469</v>
-      </c>
       <c r="Q17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="R17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="S17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="T17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="U17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="V17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="W17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="X17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.03812980651855469</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.5</v>
+        <v>0.1412894725799561</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AH17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AI17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AJ17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AK17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AL17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AM17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AN17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AO17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AP17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AQ17" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>0.9444444444444445</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>turn off the over.</t>
+          <t>turn off the oven</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>turn off the over</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="P18" t="n">
-        <v>0.03943061828613281</v>
-      </c>
       <c r="Q18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="R18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="S18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="T18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="U18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="V18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="W18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="X18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.03943061828613281</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.5</v>
+        <v>0.1481602191925049</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AH18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AI18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AJ18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AK18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AL18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AM18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AN18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AO18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AP18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AQ18" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.9444444444444445</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>0.9444444444444445</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>oven the gate.</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3400,313 +3490,323 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
+          <t>open the gate</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>oven the gate</t>
-        </is>
-      </c>
-      <c r="P19" t="n">
-        <v>0.04040956497192383</v>
+          <t>open the gate</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>open the gate</t>
+        </is>
       </c>
       <c r="Q19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="R19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="S19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="T19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="U19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="V19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="W19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="X19" t="n">
-        <v>0.04040956497192383</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.04138493537902832</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.04138493537902832</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.04138493537902832</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.04138493537902832</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.04138493537902832</v>
+        <v>0.103325366973877</v>
       </c>
       <c r="AD19" t="n">
+        <v>0.103325366973877</v>
+      </c>
+      <c r="AE19" t="n">
         <v>0.8</v>
       </c>
-      <c r="AE19" t="n">
-        <v>0.9333333333333332</v>
-      </c>
       <c r="AF19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AH19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AI19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AJ19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AK19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AL19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AM19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AN19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AO19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AP19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AQ19" t="n">
-        <v>0.9333333333333332</v>
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0.9166666666666667</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>clause the gate.</t>
+          <t>close the gate</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>clause the gate</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="P20" t="n">
-        <v>0.08374547958374023</v>
-      </c>
       <c r="Q20" t="n">
-        <v>0.08374547958374023</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="R20" t="n">
-        <v>0.08374547958374023</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="S20" t="n">
-        <v>0.08374547958374023</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="T20" t="n">
-        <v>0.08374547958374023</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="U20" t="n">
-        <v>0.08374547958374023</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="V20" t="n">
-        <v>0.08472180366516113</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="W20" t="n">
-        <v>0.08569741249084473</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="X20" t="n">
-        <v>0.08569741249084473</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.08569741249084473</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.08569741249084473</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.08569741249084473</v>
+        <v>0.1079106330871582</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.08569741249084473</v>
+        <v>0.1091368198394775</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.08569741249084473</v>
+        <v>0.1091368198394775</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.6857142857142857</v>
+        <v>0.1091368198394775</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AI20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AJ20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AK20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AL20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AM20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AN20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AO20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AP20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
       </c>
       <c r="AQ20" t="n">
-        <v>0.8777777777777778</v>
+        <v>0.9111111111111112</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>0.9111111111111112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update main.py, modify the levenshtein.py, add server.py, make new output2.xlsx
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -737,46 +737,46 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="R2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="S2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="T2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="U2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="V2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="W2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="X2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.01084661483764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.01182317733764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.01182317733764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.01182317733764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.01182317733764648</v>
+        <v>0.02636361122131348</v>
       </c>
       <c r="AE2" t="n">
         <v>0.8333333333333334</v>
@@ -903,46 +903,46 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="R3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="S3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="T3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="U3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="V3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="W3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="X3" t="n">
-        <v>0.02137184143066406</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.02234387397766113</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.02331852912902832</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.02331852912902832</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.02331852912902832</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.02331852912902832</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.02331852912902832</v>
+        <v>0.03515195846557617</v>
       </c>
       <c r="AE3" t="n">
         <v>0.9444444444444445</v>
@@ -1069,46 +1069,46 @@
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>0.02234458923339844</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="R4" t="n">
-        <v>0.02234458923339844</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="S4" t="n">
-        <v>0.02234458923339844</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="T4" t="n">
-        <v>0.02234458923339844</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="U4" t="n">
-        <v>0.02234458923339844</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="V4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="W4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="X4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.02284574508666992</v>
+        <v>0.02929973602294922</v>
       </c>
       <c r="AE4" t="n">
         <v>0.875</v>
@@ -1235,46 +1235,46 @@
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="R5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="S5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="T5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="U5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="V5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="W5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="X5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.02872991561889648</v>
+        <v>0.03518247604370117</v>
       </c>
       <c r="AE5" t="n">
         <v>0.9166666666666667</v>
@@ -1401,46 +1401,46 @@
         </is>
       </c>
       <c r="Q6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="R6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="S6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="T6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="U6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="V6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="W6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="X6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.04895639419555664</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.04995179176330566</v>
+        <v>0.06842136383056641</v>
       </c>
       <c r="AE6" t="n">
         <v>0.8666666666666667</v>
@@ -1567,46 +1567,46 @@
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05885457992553711</v>
       </c>
       <c r="R7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05885457992553711</v>
       </c>
       <c r="S7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="T7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="U7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="V7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="W7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="X7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.03751754760742188</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.03849315643310547</v>
+        <v>0.05984210968017578</v>
       </c>
       <c r="AE7" t="n">
         <v>0.875</v>
@@ -1733,46 +1733,46 @@
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="R8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="S8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="T8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="U8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="V8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="W8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="X8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06568002700805664</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06664466857910156</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.04352903366088867</v>
+        <v>0.06666874885559082</v>
       </c>
       <c r="AE8" t="n">
         <v>0.9166666666666667</v>
@@ -1899,46 +1899,46 @@
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1064484119415283</v>
       </c>
       <c r="R9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1064484119415283</v>
       </c>
       <c r="S9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1064484119415283</v>
       </c>
       <c r="T9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="U9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1064484119415283</v>
       </c>
       <c r="V9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="W9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="X9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.07251381874084473</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.0730125904083252</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.0730125904083252</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.0730125904083252</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.0730125904083252</v>
+        <v>0.1074256896972656</v>
       </c>
       <c r="AE9" t="n">
         <v>0.8333333333333334</v>
@@ -2065,46 +2065,46 @@
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1143500804901123</v>
       </c>
       <c r="R10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="S10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="T10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="U10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="V10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="W10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="X10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.08415317535400391</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.08536219596862793</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.08536219596862793</v>
+        <v>0.1151974201202393</v>
       </c>
       <c r="AE10" t="n">
         <v>0.8333333333333334</v>
@@ -2231,46 +2231,46 @@
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>0.09165453910827637</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="R11" t="n">
-        <v>0.09165453910827637</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="S11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="T11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="U11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="V11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="W11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="X11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.09262895584106445</v>
+        <v>0.1244637966156006</v>
       </c>
       <c r="AE11" t="n">
         <v>1</v>
@@ -2397,46 +2397,46 @@
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.09470272064208984</v>
       </c>
       <c r="R12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.09470272064208984</v>
       </c>
       <c r="S12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="T12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="U12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.09470272064208984</v>
       </c>
       <c r="V12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="W12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="X12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.06710195541381836</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.06758332252502441</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.06758332252502441</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.06758332252502441</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.06758332252502441</v>
+        <v>0.0956730842590332</v>
       </c>
       <c r="AE12" t="n">
         <v>0.9166666666666667</v>
@@ -2563,46 +2563,46 @@
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1498477458953857</v>
       </c>
       <c r="R13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1498477458953857</v>
       </c>
       <c r="S13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1498477458953857</v>
       </c>
       <c r="T13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="U13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1498477458953857</v>
       </c>
       <c r="V13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="W13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="X13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.109529972076416</v>
+        <v>0.1508252620697021</v>
       </c>
       <c r="AE13" t="n">
         <v>0.9583333333333334</v>
@@ -2729,46 +2729,46 @@
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="R14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="S14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="T14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="U14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="V14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="W14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="X14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.1576809883117676</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.158677339553833</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.118302583694458</v>
+        <v>0.158677339553833</v>
       </c>
       <c r="AE14" t="n">
         <v>0.9444444444444445</v>
@@ -2895,46 +2895,46 @@
         </is>
       </c>
       <c r="Q15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="R15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="S15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="T15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="U15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="V15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="W15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="X15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1094305515289307</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.08279895782470703</v>
+        <v>0.1104245185852051</v>
       </c>
       <c r="AE15" t="n">
         <v>0.875</v>
@@ -3061,46 +3061,46 @@
         </is>
       </c>
       <c r="Q16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1152205467224121</v>
       </c>
       <c r="R16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1152205467224121</v>
       </c>
       <c r="S16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1152205467224121</v>
       </c>
       <c r="T16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1152205467224121</v>
       </c>
       <c r="U16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1152205467224121</v>
       </c>
       <c r="V16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1152205467224121</v>
       </c>
       <c r="W16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="X16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.09022045135498047</v>
+        <v>0.1162075996398926</v>
       </c>
       <c r="AE16" t="n">
         <v>0.9166666666666667</v>
@@ -3227,46 +3227,46 @@
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="R17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="S17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="T17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="U17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="V17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="W17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="X17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.1412894725799561</v>
+        <v>0.192859411239624</v>
       </c>
       <c r="AE17" t="n">
         <v>0.8666666666666667</v>
@@ -3393,46 +3393,46 @@
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="R18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="S18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="T18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="U18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="V18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="W18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="X18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.201521635055542</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.2020206451416016</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.1481602191925049</v>
+        <v>0.2020206451416016</v>
       </c>
       <c r="AE18" t="n">
         <v>0.8666666666666667</v>
@@ -3559,46 +3559,46 @@
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="R19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="S19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="T19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="U19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="V19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="W19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="X19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.103325366973877</v>
+        <v>0.1389584541320801</v>
       </c>
       <c r="AE19" t="n">
         <v>0.8</v>
@@ -3725,46 +3725,46 @@
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="R20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="S20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="T20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="U20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="V20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="W20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="X20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1437268257141113</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.1079106330871582</v>
+        <v>0.1445889472961426</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.1091368198394775</v>
+        <v>0.1445889472961426</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.1091368198394775</v>
+        <v>0.1445889472961426</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.1091368198394775</v>
+        <v>0.1445889472961426</v>
       </c>
       <c r="AE20" t="n">
         <v>0.7857142857142857</v>

</xml_diff>

<commit_message>
modify several algorithm, main.py, server.py
server.py : adding GET, logic isDistance for distance algorithm

cosine, euclidien, manhattan, levenshtein : adding counter to split again in their function

longestCommon.py : change the output to returns score instead string
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR20"/>
+  <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,150 +506,135 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>N-Gram Corrected</t>
+          <t>Smith Waterman Corrected</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Smith Waterman Corrected</t>
+          <t>Jaccard Time</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Jaccard Time</t>
+          <t>JaroDistance Time</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>JaroDistance Time</t>
+          <t>Dice Coefficien Time</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Dice Coefficien Time</t>
+          <t>Cosine Time</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Cosine Time</t>
+          <t>Damerau-Levenshtein Time</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Damerau-Levenshtein Time</t>
+          <t>Euclidien Distance Time</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Euclidien Distance Time</t>
+          <t>hamming Distance Time</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>hamming Distance Time</t>
+          <t>Jaro-Winkler Time</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Jaro-Winkler Time</t>
+          <t>Longest Common Time</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Longest Common Time</t>
+          <t>Levenshtein Distance Time</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Levenshtein Distance Time</t>
+          <t>Manhattan Time</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Manhattan Time</t>
+          <t>Needleman Time</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Needleman Time</t>
+          <t>Smith Waterman Time</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>N-Gram Time</t>
+          <t>Jaccard Accuracy</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Smith Waterman Time</t>
+          <t>JaroDistance Accuracy</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Jaccard Accuracy</t>
+          <t>Dice Coefficien Accuracy</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>JaroDistance Accuracy</t>
+          <t>Cosine Accuracy</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Dice Coefficien Accuracy</t>
+          <t>Damerau-Levenshtein Accuracy</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Cosine Accuracy</t>
+          <t>Euclidien Distance Accuracy</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Damerau-Levenshtein Accuracy</t>
+          <t>hamming Distance Accuracy</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Euclidien Distance Accuracy</t>
+          <t>Jaro-Winkler Accuracy</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>hamming Distance Accuracy</t>
+          <t>Longest Common Accuracy</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Jaro-Winkler Accuracy</t>
+          <t>Levenshtein Distance Accuracy</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>Longest Common Accuracy</t>
+          <t>Manhattan Accuracy</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>Levenshtein Distance Accuracy</t>
+          <t>Needleman Accuracy</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Manhattan Accuracy</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>Needleman Accuracy</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>N-Gram Accuracy</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Smith Waterman Accuracy</t>
         </is>
@@ -673,152 +658,141 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>on turn the on</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>turn on the the</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>turn on the the</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>turn on the tv</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>turn on the tv</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>turn on the tv</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>turn on the tv</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>turn on the tv</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>turn on the tv</t>
-        </is>
-      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>turn on the tv</t>
+          <t>on turn the on</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>turn on the tv</t>
+          <t>on the the on</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>turn on the tv</t>
+          <t>turn on the the</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>turn on the tv</t>
+          <t>turn on the turn</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>turn on the tv</t>
+          <t>turn on the the</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>turn on the tv</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>turn on the tv</t>
-        </is>
+          <t>turn on the the</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>0.01173806190490723</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="R2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="S2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="T2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="U2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="V2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="W2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="X2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.01173806190490723</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.0136723518371582</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.0136723518371582</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.0136723518371582</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.0136723518371582</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.02636361122131348</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.8703703703703703</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.8703703703703703</v>
+        <v>2</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.8703703703703703</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.8703703703703703</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.8703703703703703</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.8703703703703703</v>
+        <v>7.333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -839,152 +813,141 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>off turn the turn</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>turn off the off</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>off turn the turn</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>off turn the turn</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>turn off the light</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>turn off the light</t>
-        </is>
+      <c r="P3" t="n">
+        <v>0.02470588684082031</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="R3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="S3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="T3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="U3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="V3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="W3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="X3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02470588684082031</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02779579162597656</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02779579162597656</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02779579162597656</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.02779579162597656</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.03515195846557617</v>
+        <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.9696969696969697</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.9814814814814815</v>
+        <v>1</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.9814814814814815</v>
+        <v>0</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.9814814814814815</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.9814814814814815</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0.9814814814814815</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0.9814814814814815</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>0.9814814814814815</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -1005,152 +968,141 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>lock the door</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>lock the door</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>lock the door</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>lock the door</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>lock the door</t>
-        </is>
+      <c r="P4" t="n">
+        <v>0.02547717094421387</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02547717094421387</v>
       </c>
       <c r="R4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02547717094421387</v>
       </c>
       <c r="S4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02645444869995117</v>
       </c>
       <c r="T4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02547717094421387</v>
       </c>
       <c r="U4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02645444869995117</v>
       </c>
       <c r="V4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02645444869995117</v>
       </c>
       <c r="W4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02645444869995117</v>
       </c>
       <c r="X4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02656269073486328</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02934527397155762</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.02934527397155762</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.0303337574005127</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.0303337574005127</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0.875</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.02929973602294922</v>
+        <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.875</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.9166666666666667</v>
+        <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.9166666666666667</v>
+        <v>0</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.9166666666666667</v>
+        <v>1</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.9166666666666667</v>
+        <v>3</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>0.9166666666666667</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="5">
@@ -1171,152 +1123,141 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>unlock the door</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>unlock the door</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>unlock the door</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>unlock the door</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>unlock the door</t>
-        </is>
+      <c r="P5" t="n">
+        <v>0.04220771789550781</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="R5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="S5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="T5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="U5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="V5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="W5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="X5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.04220771789550781</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.0431826114654541</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.0431826114654541</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.0431826114654541</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.0431826114654541</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.03518247604370117</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.9545454545454546</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.9444444444444444</v>
+        <v>0</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.9444444444444444</v>
+        <v>0</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.9444444444444444</v>
+        <v>4</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0.9444444444444444</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="6">
@@ -1337,152 +1278,141 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>on turn the on</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>on turn the on</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>lamp the the on</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>turn on the lamp</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>turn on the lamp</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>turn on the lamp</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>turn on the lamp</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>turn on the lamp</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>turn on the lamp</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>turn on the lamp</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>turn on the lamp</t>
-        </is>
+      <c r="P6" t="n">
+        <v>0.07700324058532715</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="R6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="S6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="T6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="U6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="V6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="W6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="X6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.07700324058532715</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.08095622062683105</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.08095622062683105</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.08095622062683105</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.08095622062683105</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.06842136383056641</v>
+        <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.9444444444444445</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>0.9444444444444445</v>
+        <v>8.333333333333334</v>
       </c>
     </row>
     <row r="7">
@@ -1503,152 +1433,141 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>the the lock</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>the the lock</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>lock the windows</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>lock the windows</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>lock the windows</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>lock the windows</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>lock the windows</t>
-        </is>
+      <c r="P7" t="n">
+        <v>0.06674957275390625</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.05885457992553711</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="R7" t="n">
-        <v>0.05885457992553711</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="S7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="T7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="U7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="V7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="W7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="X7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06674957275390625</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06869387626647949</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06869387626647949</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06869387626647949</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.06869387626647949</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0.875</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.05984210968017578</v>
+        <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.875</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.9166666666666667</v>
+        <v>0</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.9166666666666667</v>
+        <v>0</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.9166666666666667</v>
+        <v>1</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.9166666666666667</v>
+        <v>4.5</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AR7" t="n">
-        <v>0.9166666666666667</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -1669,152 +1588,141 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>the the the</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>unlock the windows</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>unlock the windows</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>unlock the windows</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>unlock the windows</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>unlock the windows</t>
-        </is>
+      <c r="P8" t="n">
+        <v>0.07455301284790039</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="S8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="T8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="U8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="V8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="W8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="X8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07455301284790039</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07653307914733887</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07653307914733887</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07653307914733887</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.06568002700805664</v>
+        <v>0.07653307914733887</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.06664466857910156</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.06666874885559082</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.9545454545454546</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.9444444444444444</v>
+        <v>0</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.9444444444444444</v>
+        <v>0</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.9444444444444444</v>
+        <v>5.5</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AR8" t="n">
-        <v>0.9444444444444444</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -1835,152 +1743,141 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>on turn the on</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>on turn the on</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>on the the the</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>turn on the fan</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>turn on the fan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>turn on the fan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>turn on the fan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>turn on the fan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>turn on the fan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>turn on the fan</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>turn on the fan</t>
-        </is>
+      <c r="P9" t="n">
+        <v>0.1230580806732178</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.1064484119415283</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1064484119415283</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1064484119415283</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="U9" t="n">
-        <v>0.1064484119415283</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="W9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.1230580806732178</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.124032735824585</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.124032735824585</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.124032735824585</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.124032735824585</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.1074256896972656</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.9259259259259259</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.9259259259259259</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>0.9259259259259259</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>0.9259259259259259</v>
-      </c>
-      <c r="AR9" t="n">
-        <v>0.9259259259259259</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -2001,152 +1898,141 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>off turn the off</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>off turn the off</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>off turn the off</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>turn off the fan</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>turn off the fan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>turn off the fan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>turn off the fan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>turn off the fan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>turn off the fan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>turn off the fan</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>turn off the fan</t>
-        </is>
+      <c r="P10" t="n">
+        <v>0.1417388916015625</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1143500804901123</v>
+        <v>0.1417388916015625</v>
       </c>
       <c r="R10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.1417388916015625</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.14298415184021</v>
       </c>
       <c r="T10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.1417388916015625</v>
       </c>
       <c r="U10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.14298415184021</v>
       </c>
       <c r="V10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.14298415184021</v>
       </c>
       <c r="W10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.14298415184021</v>
       </c>
       <c r="X10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.14298415184021</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.1491560935974121</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.15024733543396</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.15024733543396</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.15024733543396</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.1151974201202393</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0</v>
       </c>
       <c r="AK10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0</v>
       </c>
       <c r="AL10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN10" t="n">
-        <v>0.9259259259259259</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.9259259259259259</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>0.9259259259259259</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>0.9259259259259259</v>
-      </c>
-      <c r="AR10" t="n">
-        <v>0.9259259259259259</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -2167,152 +2053,141 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>on turn the turn</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>turn on the heater</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>turn on the heater</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>turn on the on</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>on turn the turn</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>on the the on</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>turn on the heater</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>turn on the heater</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>turn on the heater</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>turn on the heater</t>
-        </is>
+      <c r="P11" t="n">
+        <v>0.1636464595794678</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1637554168701172</v>
       </c>
       <c r="R11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1637554168701172</v>
       </c>
       <c r="S11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1647465229034424</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1637554168701172</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1647465229034424</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1647465229034424</v>
       </c>
       <c r="W11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1647465229034424</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1647465229034424</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1657235622406006</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1657235622406006</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1657235622406006</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0.1657235622406006</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.1244637966156006</v>
+        <v>1</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.1244637966156006</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
         <v>1</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM11" t="n">
-        <v>0.9592592592592593</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN11" t="n">
-        <v>0.9592592592592593</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.9592592592592593</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>0.9592592592592593</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>0.9592592592592593</v>
-      </c>
-      <c r="AR11" t="n">
-        <v>0.9592592592592593</v>
+        <v>10.33333333333333</v>
       </c>
     </row>
     <row r="12">
@@ -2333,152 +2208,141 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>the the enable</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>enable the heater</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>enable the enable</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>enable the heater</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>enable the enable</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>enable the the</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>the the enable</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>the the enable</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>enable the heater</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>enable the enable</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
         <is>
           <t>enable the heater</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>enable the heater</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>enable the heater</t>
-        </is>
+      <c r="P12" t="n">
+        <v>0.1163511276245117</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.09470272064208984</v>
+        <v>0.1163511276245117</v>
       </c>
       <c r="R12" t="n">
-        <v>0.09470272064208984</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="S12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="U12" t="n">
-        <v>0.09470272064208984</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="V12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="W12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="X12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.1173274517059326</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.0956730842590332</v>
+        <v>0.2888888888888889</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.9545454545454546</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.8833333333333334</v>
+        <v>0</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.8833333333333334</v>
+        <v>1</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.8833333333333334</v>
+        <v>1.414213562373095</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.8833333333333334</v>
+        <v>2</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.8833333333333334</v>
+        <v>0.2888888888888889</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.8833333333333334</v>
+        <v>1.5</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.8833333333333334</v>
+        <v>1</v>
       </c>
       <c r="AM12" t="n">
-        <v>0.8833333333333334</v>
+        <v>2</v>
       </c>
       <c r="AN12" t="n">
-        <v>0.8833333333333334</v>
+        <v>4</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.8833333333333334</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>0.8833333333333334</v>
-      </c>
-      <c r="AQ12" t="n">
-        <v>0.8833333333333334</v>
-      </c>
-      <c r="AR12" t="n">
-        <v>0.8833333333333334</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -2499,152 +2363,141 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>back the the the</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>back the the the</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>the the the the</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>disable the back door</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>disable the back door</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>disable the back door</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>disable the back door</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>disable the back door</t>
-        </is>
+      <c r="P13" t="n">
+        <v>0.1941971778869629</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.1498477458953857</v>
+        <v>0.1941971778869629</v>
       </c>
       <c r="R13" t="n">
-        <v>0.1498477458953857</v>
+        <v>0.1962089538574219</v>
       </c>
       <c r="S13" t="n">
-        <v>0.1498477458953857</v>
+        <v>0.1971817016601562</v>
       </c>
       <c r="T13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.1962089538574219</v>
       </c>
       <c r="U13" t="n">
-        <v>0.1498477458953857</v>
+        <v>0.1971817016601562</v>
       </c>
       <c r="V13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.1971817016601562</v>
       </c>
       <c r="W13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.1971817016601562</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.1971817016601562</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.2014446258544922</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.2014446258544922</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.2024197578430176</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.2024197578430176</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.1508252620697021</v>
+        <v>0.148989898989899</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.9777777777777779</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.9437229437229436</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.9437229437229436</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.9437229437229436</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.9437229437229436</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0.9437229437229436</v>
+        <v>0.148989898989899</v>
       </c>
       <c r="AK13" t="n">
-        <v>0.9437229437229436</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AL13" t="n">
-        <v>0.9437229437229436</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AM13" t="n">
-        <v>0.9437229437229436</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN13" t="n">
-        <v>0.9437229437229436</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="AO13" t="n">
-        <v>0.9437229437229436</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>0.9437229437229436</v>
-      </c>
-      <c r="AQ13" t="n">
-        <v>0.9437229437229436</v>
-      </c>
-      <c r="AR13" t="n">
-        <v>0.9437229437229436</v>
+        <v>12.33333333333333</v>
       </c>
     </row>
     <row r="14">
@@ -2665,152 +2518,141 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>the the the the</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>the the the the</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>the the the the</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>unlock the back door</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>unlock the back door</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>unlock the back door</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>unlock the back door</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>unlock the back door</t>
-        </is>
+      <c r="P14" t="n">
+        <v>0.2170569896697998</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="R14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="S14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="T14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="U14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="V14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="W14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2170569896697998</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2199840545654297</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2199840545654297</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2199840545654297</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.1576809883117676</v>
+        <v>0.2199840545654297</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.158677339553833</v>
+        <v>0.9444444444444445</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.158677339553833</v>
+        <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.9696969696969697</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AJ14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0</v>
       </c>
       <c r="AK14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0</v>
       </c>
       <c r="AL14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM14" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN14" t="n">
-        <v>0.9629629629629629</v>
+        <v>4</v>
       </c>
       <c r="AO14" t="n">
-        <v>0.9629629629629629</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>0.9629629629629629</v>
-      </c>
-      <c r="AQ14" t="n">
-        <v>0.9629629629629629</v>
-      </c>
-      <c r="AR14" t="n">
-        <v>0.9629629629629629</v>
+        <v>12.33333333333333</v>
       </c>
     </row>
     <row r="15">
@@ -2831,152 +2673,141 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>the the lock</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>the the lock</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>the the lock</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>lock the gate</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>lock the gate</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>lock the gate</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>lock the gate</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>lock the gate</t>
-        </is>
+      <c r="P15" t="n">
+        <v>0.1525149345397949</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.1525149345397949</v>
       </c>
       <c r="R15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.1525149345397949</v>
       </c>
       <c r="S15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.1525149345397949</v>
       </c>
       <c r="T15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.1525149345397949</v>
       </c>
       <c r="U15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.1525149345397949</v>
       </c>
       <c r="V15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.1525149345397949</v>
       </c>
       <c r="W15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.1525149345397949</v>
       </c>
       <c r="X15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.153519868850708</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.153519868850708</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.153519868850708</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.153519868850708</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.153519868850708</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.1094305515289307</v>
+        <v>0.875</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.1104245185852051</v>
+        <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.875</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AH15" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AJ15" t="n">
-        <v>0.9166666666666667</v>
+        <v>0</v>
       </c>
       <c r="AK15" t="n">
-        <v>0.9166666666666667</v>
+        <v>0</v>
       </c>
       <c r="AL15" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AM15" t="n">
-        <v>0.9166666666666667</v>
+        <v>1</v>
       </c>
       <c r="AN15" t="n">
-        <v>0.9166666666666667</v>
+        <v>3</v>
       </c>
       <c r="AO15" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AP15" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AQ15" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AR15" t="n">
-        <v>0.9166666666666667</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="16">
@@ -2997,152 +2828,141 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>the the unlock</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>the the unlock</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>the the unlock</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>unlock the gate</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>unlock the gate</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>unlock the gate</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>unlock the gate</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>unlock the gate</t>
-        </is>
+      <c r="P16" t="n">
+        <v>0.1703476905822754</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1152205467224121</v>
+        <v>0.1703476905822754</v>
       </c>
       <c r="R16" t="n">
-        <v>0.1152205467224121</v>
+        <v>0.1703476905822754</v>
       </c>
       <c r="S16" t="n">
-        <v>0.1152205467224121</v>
+        <v>0.1703476905822754</v>
       </c>
       <c r="T16" t="n">
-        <v>0.1152205467224121</v>
+        <v>0.1703476905822754</v>
       </c>
       <c r="U16" t="n">
-        <v>0.1152205467224121</v>
+        <v>0.1703476905822754</v>
       </c>
       <c r="V16" t="n">
-        <v>0.1152205467224121</v>
+        <v>0.1703476905822754</v>
       </c>
       <c r="W16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0.1703476905822754</v>
       </c>
       <c r="X16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0.171323299407959</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0.171323299407959</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0.171323299407959</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0.171323299407959</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0.171323299407959</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.1162075996398926</v>
+        <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.9545454545454546</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI16" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AJ16" t="n">
-        <v>0.9444444444444444</v>
+        <v>0</v>
       </c>
       <c r="AK16" t="n">
-        <v>0.9444444444444444</v>
+        <v>0</v>
       </c>
       <c r="AL16" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="AM16" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="AN16" t="n">
-        <v>0.9444444444444444</v>
+        <v>4</v>
       </c>
       <c r="AO16" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AQ16" t="n">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AR16" t="n">
-        <v>0.9444444444444444</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="17">
@@ -3163,152 +2983,141 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>on turn the turn</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>turn on the on</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>on turn the turn</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>on the the turn</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>turn on the turn</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="O17" t="inlineStr">
         <is>
           <t>turn on the oven</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>turn on the oven</t>
-        </is>
+      <c r="P17" t="n">
+        <v>0.2700502872467041</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.2700502872467041</v>
       </c>
       <c r="R17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.27130126953125</v>
       </c>
       <c r="S17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.27130126953125</v>
       </c>
       <c r="T17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.27130126953125</v>
       </c>
       <c r="U17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.27130126953125</v>
       </c>
       <c r="V17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.27130126953125</v>
       </c>
       <c r="W17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.27130126953125</v>
       </c>
       <c r="X17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.27130126953125</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.2732930183410645</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.2732930183410645</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.2732930183410645</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.2742705345153809</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.192859411239624</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AJ17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AK17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AL17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM17" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN17" t="n">
-        <v>0.9444444444444445</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="AO17" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AQ17" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AR17" t="n">
-        <v>0.9444444444444445</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -3329,152 +3138,141 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>off turn the turn</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>off turn the turn</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>off turn the turn</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>turn off the turn</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>turn off the oven</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>turn off the oven</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>turn off the oven</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>turn off the oven</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>turn off the oven</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>turn off the oven</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>turn off the oven</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>turn off the oven</t>
-        </is>
+      <c r="P18" t="n">
+        <v>0.2989897727966309</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.2989897727966309</v>
       </c>
       <c r="R18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.2989897727966309</v>
       </c>
       <c r="S18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3009510040283203</v>
       </c>
       <c r="T18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.2989897727966309</v>
       </c>
       <c r="U18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3009510040283203</v>
       </c>
       <c r="V18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3009510040283203</v>
       </c>
       <c r="W18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3009510040283203</v>
       </c>
       <c r="X18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3009510040283203</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3038690090179443</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3038690090179443</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3038690090179443</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.201521635055542</v>
+        <v>0.3038690090179443</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.2020206451416016</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.2020206451416016</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AH18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.4714045207910317</v>
       </c>
       <c r="AI18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AJ18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AK18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AL18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM18" t="n">
-        <v>0.9444444444444445</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN18" t="n">
-        <v>0.9444444444444445</v>
+        <v>3</v>
       </c>
       <c r="AO18" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AP18" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AQ18" t="n">
-        <v>0.9444444444444445</v>
-      </c>
-      <c r="AR18" t="n">
-        <v>0.9444444444444445</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -3495,152 +3293,141 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>gate the open</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>gate the open</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>the the open</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="O19" t="inlineStr">
         <is>
           <t>open the gate</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>open the gate</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>open the gate</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>open the gate</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>open the gate</t>
-        </is>
+      <c r="P19" t="n">
+        <v>0.2100651264190674</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="R19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="S19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="T19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="U19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="V19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="W19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="X19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2100651264190674</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2110400199890137</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.2110400199890137</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.8</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.1389584541320801</v>
+        <v>0.5</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.8</v>
+        <v>0.875</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AH19" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI19" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AJ19" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AK19" t="n">
-        <v>0.9166666666666667</v>
+        <v>1</v>
       </c>
       <c r="AL19" t="n">
-        <v>0.9166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="AM19" t="n">
-        <v>0.9166666666666667</v>
+        <v>1</v>
       </c>
       <c r="AN19" t="n">
-        <v>0.9166666666666667</v>
+        <v>3</v>
       </c>
       <c r="AO19" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AQ19" t="n">
-        <v>0.9166666666666667</v>
-      </c>
-      <c r="AR19" t="n">
-        <v>0.9166666666666667</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="20">
@@ -3661,152 +3448,141 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>the the close</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>the the close</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>the the close</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>close the gate</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>close the gate</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>close the gate</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>close the gate</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>close the gate</t>
-        </is>
+      <c r="P20" t="n">
+        <v>0.2159242630004883</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="R20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="S20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="T20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="U20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="V20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="W20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="X20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2159242630004883</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2169032096862793</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.1437268257141113</v>
+        <v>0.2169032096862793</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.1445889472961426</v>
+        <v>0.2169032096862793</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.1445889472961426</v>
+        <v>0.2169032096862793</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.1445889472961426</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.1445889472961426</v>
+        <v>0.2416666666666667</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.7857142857142857</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.9111111111111112</v>
+        <v>0.5</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.9111111111111112</v>
+        <v>1</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.9111111111111112</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="AI20" t="n">
-        <v>0.9111111111111112</v>
+        <v>1.5</v>
       </c>
       <c r="AJ20" t="n">
-        <v>0.9111111111111112</v>
+        <v>0.2416666666666667</v>
       </c>
       <c r="AK20" t="n">
-        <v>0.9111111111111112</v>
+        <v>1</v>
       </c>
       <c r="AL20" t="n">
-        <v>0.9111111111111112</v>
+        <v>1</v>
       </c>
       <c r="AM20" t="n">
-        <v>0.9111111111111112</v>
+        <v>1</v>
       </c>
       <c r="AN20" t="n">
-        <v>0.9111111111111112</v>
+        <v>3</v>
       </c>
       <c r="AO20" t="n">
-        <v>0.9111111111111112</v>
-      </c>
-      <c r="AP20" t="n">
-        <v>0.9111111111111112</v>
-      </c>
-      <c r="AQ20" t="n">
-        <v>0.9111111111111112</v>
-      </c>
-      <c r="AR20" t="n">
-        <v>0.9111111111111112</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>